<commit_message>
Ieskats vizualizācijās un Pandas bibliotekā
</commit_message>
<xml_diff>
--- a/data/cesis.xlsx
+++ b/data/cesis.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="21">
   <si>
     <t>Mēnesis</t>
   </si>
@@ -41,9 +41,6 @@
   </si>
   <si>
     <t>Gads</t>
-  </si>
-  <si>
-    <t>F/L</t>
   </si>
   <si>
     <t>Janvāris</t>
@@ -80,9 +77,6 @@
   </si>
   <si>
     <t>Decembris</t>
-  </si>
-  <si>
-    <t>inf</t>
   </si>
 </sst>
 </file>
@@ -440,13 +434,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K73"/>
+  <dimension ref="A1:J73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:10">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -474,16 +468,13 @@
       <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2">
         <v>492</v>
@@ -492,7 +483,7 @@
         <v>110</v>
       </c>
       <c r="E2">
-        <v>586</v>
+        <v>576</v>
       </c>
       <c r="F2">
         <v>385</v>
@@ -509,16 +500,13 @@
       <c r="J2">
         <v>2014</v>
       </c>
-      <c r="K2">
-        <v>4.472727272727273</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3">
         <v>69</v>
@@ -527,7 +515,7 @@
         <v>94</v>
       </c>
       <c r="E3">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="F3">
         <v>94</v>
@@ -544,16 +532,13 @@
       <c r="J3">
         <v>2014</v>
       </c>
-      <c r="K3">
-        <v>0.7340425531914894</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4">
         <v>238</v>
@@ -562,7 +547,7 @@
         <v>348</v>
       </c>
       <c r="E4">
-        <v>267</v>
+        <v>257</v>
       </c>
       <c r="F4">
         <v>154</v>
@@ -579,16 +564,13 @@
       <c r="J4">
         <v>2014</v>
       </c>
-      <c r="K4">
-        <v>0.6839080459770115</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5">
         <v>332</v>
@@ -597,7 +579,7 @@
         <v>254</v>
       </c>
       <c r="E5">
-        <v>527</v>
+        <v>517</v>
       </c>
       <c r="F5">
         <v>258</v>
@@ -614,16 +596,13 @@
       <c r="J5">
         <v>2014</v>
       </c>
-      <c r="K5">
-        <v>1.307086614173228</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6">
         <v>1257</v>
@@ -632,7 +611,7 @@
         <v>2295</v>
       </c>
       <c r="E6">
-        <v>982</v>
+        <v>972</v>
       </c>
       <c r="F6">
         <v>673</v>
@@ -649,16 +628,13 @@
       <c r="J6">
         <v>2014</v>
       </c>
-      <c r="K6">
-        <v>0.5477124183006536</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7">
         <v>2041</v>
@@ -667,7 +643,7 @@
         <v>573</v>
       </c>
       <c r="E7">
-        <v>1421</v>
+        <v>1411</v>
       </c>
       <c r="F7">
         <v>994</v>
@@ -684,16 +660,13 @@
       <c r="J7">
         <v>2014</v>
       </c>
-      <c r="K7">
-        <v>3.56195462478185</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8">
         <v>1783</v>
@@ -702,7 +675,7 @@
         <v>572</v>
       </c>
       <c r="E8">
-        <v>3127</v>
+        <v>3117</v>
       </c>
       <c r="F8">
         <v>1599</v>
@@ -719,16 +692,13 @@
       <c r="J8">
         <v>2014</v>
       </c>
-      <c r="K8">
-        <v>3.117132867132867</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9">
         <v>2006</v>
@@ -737,7 +707,7 @@
         <v>614</v>
       </c>
       <c r="E9">
-        <v>3948</v>
+        <v>3938</v>
       </c>
       <c r="F9">
         <v>1853</v>
@@ -754,16 +724,13 @@
       <c r="J9">
         <v>2014</v>
       </c>
-      <c r="K9">
-        <v>3.267100977198697</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10">
         <v>1142</v>
@@ -772,7 +739,7 @@
         <v>599</v>
       </c>
       <c r="E10">
-        <v>1360</v>
+        <v>1350</v>
       </c>
       <c r="F10">
         <v>1036</v>
@@ -789,16 +756,13 @@
       <c r="J10">
         <v>2014</v>
       </c>
-      <c r="K10">
-        <v>1.906510851419032</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11">
         <v>531</v>
@@ -807,7 +771,7 @@
         <v>787</v>
       </c>
       <c r="E11">
-        <v>1017</v>
+        <v>1007</v>
       </c>
       <c r="F11">
         <v>454</v>
@@ -824,16 +788,13 @@
       <c r="J11">
         <v>2014</v>
       </c>
-      <c r="K11">
-        <v>0.6747141041931385</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C12">
         <v>293</v>
@@ -842,7 +803,7 @@
         <v>165</v>
       </c>
       <c r="E12">
-        <v>541</v>
+        <v>531</v>
       </c>
       <c r="F12">
         <v>292</v>
@@ -859,16 +820,13 @@
       <c r="J12">
         <v>2014</v>
       </c>
-      <c r="K12">
-        <v>1.775757575757576</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C13">
         <v>78</v>
@@ -877,7 +835,7 @@
         <v>99</v>
       </c>
       <c r="E13">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="F13">
         <v>82</v>
@@ -894,16 +852,13 @@
       <c r="J13">
         <v>2014</v>
       </c>
-      <c r="K13">
-        <v>0.7878787878787878</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C14">
         <v>224</v>
@@ -912,7 +867,7 @@
         <v>33</v>
       </c>
       <c r="E14">
-        <v>446</v>
+        <v>436</v>
       </c>
       <c r="F14">
         <v>262</v>
@@ -929,16 +884,13 @@
       <c r="J14">
         <v>2015</v>
       </c>
-      <c r="K14">
-        <v>6.787878787878788</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11">
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C15">
         <v>269</v>
@@ -947,7 +899,7 @@
         <v>89</v>
       </c>
       <c r="E15">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="F15">
         <v>172</v>
@@ -964,16 +916,13 @@
       <c r="J15">
         <v>2015</v>
       </c>
-      <c r="K15">
-        <v>3.02247191011236</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11">
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C16">
         <v>118</v>
@@ -982,7 +931,7 @@
         <v>43</v>
       </c>
       <c r="E16">
-        <v>500</v>
+        <v>490</v>
       </c>
       <c r="F16">
         <v>228</v>
@@ -999,16 +948,13 @@
       <c r="J16">
         <v>2015</v>
       </c>
-      <c r="K16">
-        <v>2.744186046511628</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11">
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C17">
         <v>497</v>
@@ -1017,7 +963,7 @@
         <v>250</v>
       </c>
       <c r="E17">
-        <v>485</v>
+        <v>475</v>
       </c>
       <c r="F17">
         <v>252</v>
@@ -1034,16 +980,13 @@
       <c r="J17">
         <v>2015</v>
       </c>
-      <c r="K17">
-        <v>1.988</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11">
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C18">
         <v>1316</v>
@@ -1052,7 +995,7 @@
         <v>769</v>
       </c>
       <c r="E18">
-        <v>1090</v>
+        <v>1080</v>
       </c>
       <c r="F18">
         <v>778</v>
@@ -1069,16 +1012,13 @@
       <c r="J18">
         <v>2015</v>
       </c>
-      <c r="K18">
-        <v>1.711313394018205</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11">
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C19">
         <v>1870</v>
@@ -1087,7 +1027,7 @@
         <v>765</v>
       </c>
       <c r="E19">
-        <v>1525</v>
+        <v>1515</v>
       </c>
       <c r="F19">
         <v>1232</v>
@@ -1104,16 +1044,13 @@
       <c r="J19">
         <v>2015</v>
       </c>
-      <c r="K19">
-        <v>2.444444444444445</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11">
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C20">
         <v>1780</v>
@@ -1122,7 +1059,7 @@
         <v>477</v>
       </c>
       <c r="E20">
-        <v>4121</v>
+        <v>4111</v>
       </c>
       <c r="F20">
         <v>2057</v>
@@ -1139,16 +1076,13 @@
       <c r="J20">
         <v>2015</v>
       </c>
-      <c r="K20">
-        <v>3.731656184486373</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11">
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C21">
         <v>1896</v>
@@ -1157,7 +1091,7 @@
         <v>197</v>
       </c>
       <c r="E21">
-        <v>2850</v>
+        <v>2840</v>
       </c>
       <c r="F21">
         <v>2107</v>
@@ -1174,16 +1108,13 @@
       <c r="J21">
         <v>2015</v>
       </c>
-      <c r="K21">
-        <v>9.624365482233502</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11">
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22" s="1">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C22">
         <v>1521</v>
@@ -1192,7 +1123,7 @@
         <v>417</v>
       </c>
       <c r="E22">
-        <v>1277</v>
+        <v>1267</v>
       </c>
       <c r="F22">
         <v>1073</v>
@@ -1209,16 +1140,13 @@
       <c r="J22">
         <v>2015</v>
       </c>
-      <c r="K22">
-        <v>3.647482014388489</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11">
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23" s="1">
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C23">
         <v>849</v>
@@ -1227,7 +1155,7 @@
         <v>623</v>
       </c>
       <c r="E23">
-        <v>1478</v>
+        <v>1468</v>
       </c>
       <c r="F23">
         <v>832</v>
@@ -1244,16 +1172,13 @@
       <c r="J23">
         <v>2015</v>
       </c>
-      <c r="K23">
-        <v>1.362760834670947</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11">
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24" s="1">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C24">
         <v>367</v>
@@ -1262,7 +1187,7 @@
         <v>167</v>
       </c>
       <c r="E24">
-        <v>529</v>
+        <v>519</v>
       </c>
       <c r="F24">
         <v>284</v>
@@ -1279,16 +1204,13 @@
       <c r="J24">
         <v>2015</v>
       </c>
-      <c r="K24">
-        <v>2.197604790419162</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11">
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25" s="1">
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C25">
         <v>116</v>
@@ -1297,7 +1219,7 @@
         <v>112</v>
       </c>
       <c r="E25">
-        <v>371</v>
+        <v>361</v>
       </c>
       <c r="F25">
         <v>210</v>
@@ -1314,16 +1236,13 @@
       <c r="J25">
         <v>2015</v>
       </c>
-      <c r="K25">
-        <v>1.035714285714286</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11">
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26" s="1">
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C26">
         <v>172</v>
@@ -1332,7 +1251,7 @@
         <v>100</v>
       </c>
       <c r="E26">
-        <v>357</v>
+        <v>347</v>
       </c>
       <c r="F26">
         <v>290</v>
@@ -1349,16 +1268,13 @@
       <c r="J26">
         <v>2016</v>
       </c>
-      <c r="K26">
-        <v>1.72</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11">
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27" s="1">
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C27">
         <v>49</v>
@@ -1367,7 +1283,7 @@
         <v>134</v>
       </c>
       <c r="E27">
-        <v>308</v>
+        <v>298</v>
       </c>
       <c r="F27">
         <v>286</v>
@@ -1384,16 +1300,13 @@
       <c r="J27">
         <v>2016</v>
       </c>
-      <c r="K27">
-        <v>0.3656716417910448</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11">
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28" s="1">
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C28">
         <v>332</v>
@@ -1402,7 +1315,7 @@
         <v>128</v>
       </c>
       <c r="E28">
-        <v>721</v>
+        <v>711</v>
       </c>
       <c r="F28">
         <v>366</v>
@@ -1419,16 +1332,13 @@
       <c r="J28">
         <v>2016</v>
       </c>
-      <c r="K28">
-        <v>2.59375</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11">
+    </row>
+    <row r="29" spans="1:10">
       <c r="A29" s="1">
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C29">
         <v>609</v>
@@ -1437,7 +1347,7 @@
         <v>225</v>
       </c>
       <c r="E29">
-        <v>645</v>
+        <v>635</v>
       </c>
       <c r="F29">
         <v>446</v>
@@ -1454,16 +1364,13 @@
       <c r="J29">
         <v>2016</v>
       </c>
-      <c r="K29">
-        <v>2.706666666666667</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11">
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30" s="1">
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C30">
         <v>1442</v>
@@ -1472,7 +1379,7 @@
         <v>330</v>
       </c>
       <c r="E30">
-        <v>1415</v>
+        <v>1405</v>
       </c>
       <c r="F30">
         <v>1158</v>
@@ -1489,16 +1396,13 @@
       <c r="J30">
         <v>2016</v>
       </c>
-      <c r="K30">
-        <v>4.36969696969697</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11">
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31" s="1">
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C31">
         <v>2300</v>
@@ -1507,7 +1411,7 @@
         <v>322</v>
       </c>
       <c r="E31">
-        <v>1803</v>
+        <v>1793</v>
       </c>
       <c r="F31">
         <v>1515</v>
@@ -1524,16 +1428,13 @@
       <c r="J31">
         <v>2016</v>
       </c>
-      <c r="K31">
-        <v>7.142857142857143</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11">
+    </row>
+    <row r="32" spans="1:10">
       <c r="A32" s="1">
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C32">
         <v>2047</v>
@@ -1542,7 +1443,7 @@
         <v>652</v>
       </c>
       <c r="E32">
-        <v>4689</v>
+        <v>4679</v>
       </c>
       <c r="F32">
         <v>3041</v>
@@ -1559,16 +1460,13 @@
       <c r="J32">
         <v>2016</v>
       </c>
-      <c r="K32">
-        <v>3.139570552147239</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11">
+    </row>
+    <row r="33" spans="1:10">
       <c r="A33" s="1">
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C33">
         <v>1879</v>
@@ -1577,7 +1475,7 @@
         <v>502</v>
       </c>
       <c r="E33">
-        <v>4495</v>
+        <v>4485</v>
       </c>
       <c r="F33">
         <v>2970</v>
@@ -1594,16 +1492,13 @@
       <c r="J33">
         <v>2016</v>
       </c>
-      <c r="K33">
-        <v>3.743027888446215</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11">
+    </row>
+    <row r="34" spans="1:10">
       <c r="A34" s="1">
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C34">
         <v>1525</v>
@@ -1612,7 +1507,7 @@
         <v>733</v>
       </c>
       <c r="E34">
-        <v>1359</v>
+        <v>1349</v>
       </c>
       <c r="F34">
         <v>1284</v>
@@ -1629,16 +1524,13 @@
       <c r="J34">
         <v>2016</v>
       </c>
-      <c r="K34">
-        <v>2.080491132332879</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11">
+    </row>
+    <row r="35" spans="1:10">
       <c r="A35" s="1">
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C35">
         <v>535</v>
@@ -1647,7 +1539,7 @@
         <v>518</v>
       </c>
       <c r="E35">
-        <v>1253</v>
+        <v>1243</v>
       </c>
       <c r="F35">
         <v>847</v>
@@ -1664,16 +1556,13 @@
       <c r="J35">
         <v>2016</v>
       </c>
-      <c r="K35">
-        <v>1.032818532818533</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11">
+    </row>
+    <row r="36" spans="1:10">
       <c r="A36" s="1">
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C36">
         <v>255</v>
@@ -1682,7 +1571,7 @@
         <v>95</v>
       </c>
       <c r="E36">
-        <v>297</v>
+        <v>287</v>
       </c>
       <c r="F36">
         <v>256</v>
@@ -1699,16 +1588,13 @@
       <c r="J36">
         <v>2016</v>
       </c>
-      <c r="K36">
-        <v>2.684210526315789</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11">
+    </row>
+    <row r="37" spans="1:10">
       <c r="A37" s="1">
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C37">
         <v>127</v>
@@ -1717,7 +1603,7 @@
         <v>189</v>
       </c>
       <c r="E37">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="F37">
         <v>194</v>
@@ -1734,16 +1620,13 @@
       <c r="J37">
         <v>2016</v>
       </c>
-      <c r="K37">
-        <v>0.671957671957672</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11">
+    </row>
+    <row r="38" spans="1:10">
       <c r="A38" s="1">
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C38">
         <v>176</v>
@@ -1752,7 +1635,7 @@
         <v>35</v>
       </c>
       <c r="E38">
-        <v>423</v>
+        <v>413</v>
       </c>
       <c r="F38">
         <v>356</v>
@@ -1769,16 +1652,13 @@
       <c r="J38">
         <v>2017</v>
       </c>
-      <c r="K38">
-        <v>5.028571428571428</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11">
+    </row>
+    <row r="39" spans="1:10">
       <c r="A39" s="1">
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C39">
         <v>66</v>
@@ -1787,7 +1667,7 @@
         <v>50</v>
       </c>
       <c r="E39">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F39">
         <v>312</v>
@@ -1804,16 +1684,13 @@
       <c r="J39">
         <v>2017</v>
       </c>
-      <c r="K39">
-        <v>1.32</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11">
+    </row>
+    <row r="40" spans="1:10">
       <c r="A40" s="1">
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C40">
         <v>37</v>
@@ -1822,7 +1699,7 @@
         <v>0</v>
       </c>
       <c r="E40">
-        <v>451</v>
+        <v>441</v>
       </c>
       <c r="F40">
         <v>276</v>
@@ -1839,16 +1716,13 @@
       <c r="J40">
         <v>2017</v>
       </c>
-      <c r="K40" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11">
+    </row>
+    <row r="41" spans="1:10">
       <c r="A41" s="1">
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C41">
         <v>412</v>
@@ -1857,7 +1731,7 @@
         <v>206</v>
       </c>
       <c r="E41">
-        <v>685</v>
+        <v>675</v>
       </c>
       <c r="F41">
         <v>464</v>
@@ -1874,16 +1748,13 @@
       <c r="J41">
         <v>2017</v>
       </c>
-      <c r="K41">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11">
+    </row>
+    <row r="42" spans="1:10">
       <c r="A42" s="1">
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C42">
         <v>1384</v>
@@ -1892,7 +1763,7 @@
         <v>491</v>
       </c>
       <c r="E42">
-        <v>1637</v>
+        <v>1627</v>
       </c>
       <c r="F42">
         <v>1447</v>
@@ -1909,16 +1780,13 @@
       <c r="J42">
         <v>2017</v>
       </c>
-      <c r="K42">
-        <v>2.818737270875764</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11">
+    </row>
+    <row r="43" spans="1:10">
       <c r="A43" s="1">
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C43">
         <v>1939</v>
@@ -1927,7 +1795,7 @@
         <v>599</v>
       </c>
       <c r="E43">
-        <v>1700</v>
+        <v>1690</v>
       </c>
       <c r="F43">
         <v>1824</v>
@@ -1944,16 +1812,13 @@
       <c r="J43">
         <v>2017</v>
       </c>
-      <c r="K43">
-        <v>3.237061769616027</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11">
+    </row>
+    <row r="44" spans="1:10">
       <c r="A44" s="1">
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C44">
         <v>2030</v>
@@ -1962,7 +1827,7 @@
         <v>456</v>
       </c>
       <c r="E44">
-        <v>5096</v>
+        <v>5086</v>
       </c>
       <c r="F44">
         <v>3044</v>
@@ -1979,16 +1844,13 @@
       <c r="J44">
         <v>2017</v>
       </c>
-      <c r="K44">
-        <v>4.451754385964913</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11">
+    </row>
+    <row r="45" spans="1:10">
       <c r="A45" s="1">
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C45">
         <v>2108</v>
@@ -1997,7 +1859,7 @@
         <v>709</v>
       </c>
       <c r="E45">
-        <v>4579</v>
+        <v>4569</v>
       </c>
       <c r="F45">
         <v>2960</v>
@@ -2014,16 +1876,13 @@
       <c r="J45">
         <v>2017</v>
       </c>
-      <c r="K45">
-        <v>2.973201692524682</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11">
+    </row>
+    <row r="46" spans="1:10">
       <c r="A46" s="1">
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C46">
         <v>1645</v>
@@ -2032,7 +1891,7 @@
         <v>583</v>
       </c>
       <c r="E46">
-        <v>1320</v>
+        <v>1310</v>
       </c>
       <c r="F46">
         <v>1376</v>
@@ -2049,16 +1908,13 @@
       <c r="J46">
         <v>2017</v>
       </c>
-      <c r="K46">
-        <v>2.821612349914237</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11">
+    </row>
+    <row r="47" spans="1:10">
       <c r="A47" s="1">
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C47">
         <v>663</v>
@@ -2067,7 +1923,7 @@
         <v>512</v>
       </c>
       <c r="E47">
-        <v>1349</v>
+        <v>1339</v>
       </c>
       <c r="F47">
         <v>1090</v>
@@ -2084,16 +1940,13 @@
       <c r="J47">
         <v>2017</v>
       </c>
-      <c r="K47">
-        <v>1.294921875</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11">
+    </row>
+    <row r="48" spans="1:10">
       <c r="A48" s="1">
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C48">
         <v>135</v>
@@ -2102,7 +1955,7 @@
         <v>118</v>
       </c>
       <c r="E48">
-        <v>483</v>
+        <v>473</v>
       </c>
       <c r="F48">
         <v>322</v>
@@ -2119,16 +1972,13 @@
       <c r="J48">
         <v>2017</v>
       </c>
-      <c r="K48">
-        <v>1.14406779661017</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11">
+    </row>
+    <row r="49" spans="1:10">
       <c r="A49" s="1">
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C49">
         <v>65</v>
@@ -2137,7 +1987,7 @@
         <v>83</v>
       </c>
       <c r="E49">
-        <v>411</v>
+        <v>401</v>
       </c>
       <c r="F49">
         <v>220</v>
@@ -2154,16 +2004,13 @@
       <c r="J49">
         <v>2017</v>
       </c>
-      <c r="K49">
-        <v>0.7831325301204819</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11">
+    </row>
+    <row r="50" spans="1:10">
       <c r="A50" s="1">
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C50">
         <v>269</v>
@@ -2172,7 +2019,7 @@
         <v>202</v>
       </c>
       <c r="E50">
-        <v>785</v>
+        <v>775</v>
       </c>
       <c r="F50">
         <v>604</v>
@@ -2189,16 +2036,13 @@
       <c r="J50">
         <v>2018</v>
       </c>
-      <c r="K50">
-        <v>1.331683168316832</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11">
+    </row>
+    <row r="51" spans="1:10">
       <c r="A51" s="1">
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C51">
         <v>124</v>
@@ -2207,7 +2051,7 @@
         <v>35</v>
       </c>
       <c r="E51">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="F51">
         <v>204</v>
@@ -2224,16 +2068,13 @@
       <c r="J51">
         <v>2018</v>
       </c>
-      <c r="K51">
-        <v>3.542857142857143</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11">
+    </row>
+    <row r="52" spans="1:10">
       <c r="A52" s="1">
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C52">
         <v>275</v>
@@ -2242,7 +2083,7 @@
         <v>70</v>
       </c>
       <c r="E52">
-        <v>475</v>
+        <v>465</v>
       </c>
       <c r="F52">
         <v>319</v>
@@ -2259,16 +2100,13 @@
       <c r="J52">
         <v>2018</v>
       </c>
-      <c r="K52">
-        <v>3.928571428571428</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11">
+    </row>
+    <row r="53" spans="1:10">
       <c r="A53" s="1">
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C53">
         <v>325</v>
@@ -2277,7 +2115,7 @@
         <v>44</v>
       </c>
       <c r="E53">
-        <v>629</v>
+        <v>619</v>
       </c>
       <c r="F53">
         <v>456</v>
@@ -2294,16 +2132,13 @@
       <c r="J53">
         <v>2018</v>
       </c>
-      <c r="K53">
-        <v>7.386363636363637</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11">
+    </row>
+    <row r="54" spans="1:10">
       <c r="A54" s="1">
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C54">
         <v>1225</v>
@@ -2312,7 +2147,7 @@
         <v>240</v>
       </c>
       <c r="E54">
-        <v>1369</v>
+        <v>1359</v>
       </c>
       <c r="F54">
         <v>1064</v>
@@ -2329,16 +2164,13 @@
       <c r="J54">
         <v>2018</v>
       </c>
-      <c r="K54">
-        <v>5.104166666666667</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11">
+    </row>
+    <row r="55" spans="1:10">
       <c r="A55" s="1">
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C55">
         <v>1985</v>
@@ -2347,7 +2179,7 @@
         <v>344</v>
       </c>
       <c r="E55">
-        <v>1599</v>
+        <v>1589</v>
       </c>
       <c r="F55">
         <v>1298</v>
@@ -2364,16 +2196,13 @@
       <c r="J55">
         <v>2018</v>
       </c>
-      <c r="K55">
-        <v>5.770348837209302</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11">
+    </row>
+    <row r="56" spans="1:10">
       <c r="A56" s="1">
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C56">
         <v>2119</v>
@@ -2382,7 +2211,7 @@
         <v>548</v>
       </c>
       <c r="E56">
-        <v>4199</v>
+        <v>4189</v>
       </c>
       <c r="F56">
         <v>2728</v>
@@ -2399,16 +2228,13 @@
       <c r="J56">
         <v>2018</v>
       </c>
-      <c r="K56">
-        <v>3.866788321167883</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11">
+    </row>
+    <row r="57" spans="1:10">
       <c r="A57" s="1">
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C57">
         <v>2151</v>
@@ -2417,7 +2243,7 @@
         <v>507</v>
       </c>
       <c r="E57">
-        <v>3807</v>
+        <v>3797</v>
       </c>
       <c r="F57">
         <v>3001</v>
@@ -2434,16 +2260,13 @@
       <c r="J57">
         <v>2018</v>
       </c>
-      <c r="K57">
-        <v>4.242603550295858</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11">
+    </row>
+    <row r="58" spans="1:10">
       <c r="A58" s="1">
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C58">
         <v>1779</v>
@@ -2452,7 +2275,7 @@
         <v>892</v>
       </c>
       <c r="E58">
-        <v>1013</v>
+        <v>1003</v>
       </c>
       <c r="F58">
         <v>1054</v>
@@ -2469,16 +2292,13 @@
       <c r="J58">
         <v>2018</v>
       </c>
-      <c r="K58">
-        <v>1.994394618834081</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11">
+    </row>
+    <row r="59" spans="1:10">
       <c r="A59" s="1">
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C59">
         <v>837</v>
@@ -2487,7 +2307,7 @@
         <v>496</v>
       </c>
       <c r="E59">
-        <v>1132</v>
+        <v>1122</v>
       </c>
       <c r="F59">
         <v>792</v>
@@ -2504,16 +2324,13 @@
       <c r="J59">
         <v>2018</v>
       </c>
-      <c r="K59">
-        <v>1.6875</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11">
+    </row>
+    <row r="60" spans="1:10">
       <c r="A60" s="1">
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C60">
         <v>259</v>
@@ -2522,7 +2339,7 @@
         <v>64</v>
       </c>
       <c r="E60">
-        <v>590</v>
+        <v>580</v>
       </c>
       <c r="F60">
         <v>394</v>
@@ -2539,16 +2356,13 @@
       <c r="J60">
         <v>2018</v>
       </c>
-      <c r="K60">
-        <v>4.046875</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11">
+    </row>
+    <row r="61" spans="1:10">
       <c r="A61" s="1">
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C61">
         <v>248</v>
@@ -2557,7 +2371,7 @@
         <v>240</v>
       </c>
       <c r="E61">
-        <v>348</v>
+        <v>338</v>
       </c>
       <c r="F61">
         <v>208</v>
@@ -2574,16 +2388,13 @@
       <c r="J61">
         <v>2018</v>
       </c>
-      <c r="K61">
-        <v>1.033333333333333</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11">
+    </row>
+    <row r="62" spans="1:10">
       <c r="A62" s="1">
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C62">
         <v>338</v>
@@ -2592,7 +2403,7 @@
         <v>85</v>
       </c>
       <c r="E62">
-        <v>519</v>
+        <v>509</v>
       </c>
       <c r="F62">
         <v>280</v>
@@ -2609,16 +2420,13 @@
       <c r="J62">
         <v>2019</v>
       </c>
-      <c r="K62">
-        <v>3.976470588235294</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11">
+    </row>
+    <row r="63" spans="1:10">
       <c r="A63" s="1">
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C63">
         <v>301</v>
@@ -2627,7 +2435,7 @@
         <v>125</v>
       </c>
       <c r="E63">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="F63">
         <v>182</v>
@@ -2644,16 +2452,13 @@
       <c r="J63">
         <v>2019</v>
       </c>
-      <c r="K63">
-        <v>2.408</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11">
+    </row>
+    <row r="64" spans="1:10">
       <c r="A64" s="1">
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C64">
         <v>293</v>
@@ -2662,7 +2467,7 @@
         <v>112</v>
       </c>
       <c r="E64">
-        <v>458</v>
+        <v>448</v>
       </c>
       <c r="F64">
         <v>348</v>
@@ -2679,16 +2484,13 @@
       <c r="J64">
         <v>2019</v>
       </c>
-      <c r="K64">
-        <v>2.616071428571428</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11">
+    </row>
+    <row r="65" spans="1:10">
       <c r="A65" s="1">
         <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C65">
         <v>527</v>
@@ -2697,7 +2499,7 @@
         <v>120</v>
       </c>
       <c r="E65">
-        <v>631</v>
+        <v>621</v>
       </c>
       <c r="F65">
         <v>333</v>
@@ -2714,16 +2516,13 @@
       <c r="J65">
         <v>2019</v>
       </c>
-      <c r="K65">
-        <v>4.391666666666667</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11">
+    </row>
+    <row r="66" spans="1:10">
       <c r="A66" s="1">
         <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C66">
         <v>1659</v>
@@ -2732,7 +2531,7 @@
         <v>210</v>
       </c>
       <c r="E66">
-        <v>915</v>
+        <v>905</v>
       </c>
       <c r="F66">
         <v>915</v>
@@ -2749,16 +2548,13 @@
       <c r="J66">
         <v>2019</v>
       </c>
-      <c r="K66">
-        <v>7.9</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11">
+    </row>
+    <row r="67" spans="1:10">
       <c r="A67" s="1">
         <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C67">
         <v>2091</v>
@@ -2767,7 +2563,7 @@
         <v>207</v>
       </c>
       <c r="E67">
-        <v>1538</v>
+        <v>1528</v>
       </c>
       <c r="F67">
         <v>1385</v>
@@ -2784,16 +2580,13 @@
       <c r="J67">
         <v>2019</v>
       </c>
-      <c r="K67">
-        <v>10.10144927536232</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11">
+    </row>
+    <row r="68" spans="1:10">
       <c r="A68" s="1">
         <v>66</v>
       </c>
       <c r="B68" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C68">
         <v>1753</v>
@@ -2802,7 +2595,7 @@
         <v>420</v>
       </c>
       <c r="E68">
-        <v>4007</v>
+        <v>3997</v>
       </c>
       <c r="F68">
         <v>2648</v>
@@ -2819,16 +2612,13 @@
       <c r="J68">
         <v>2019</v>
       </c>
-      <c r="K68">
-        <v>4.173809523809524</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11">
+    </row>
+    <row r="69" spans="1:10">
       <c r="A69" s="1">
         <v>67</v>
       </c>
       <c r="B69" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C69">
         <v>2114</v>
@@ -2837,7 +2627,7 @@
         <v>547</v>
       </c>
       <c r="E69">
-        <v>4981</v>
+        <v>4971</v>
       </c>
       <c r="F69">
         <v>3026</v>
@@ -2854,16 +2644,13 @@
       <c r="J69">
         <v>2019</v>
       </c>
-      <c r="K69">
-        <v>3.864716636197441</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11">
+    </row>
+    <row r="70" spans="1:10">
       <c r="A70" s="1">
         <v>68</v>
       </c>
       <c r="B70" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C70">
         <v>1369</v>
@@ -2872,7 +2659,7 @@
         <v>482</v>
       </c>
       <c r="E70">
-        <v>1121</v>
+        <v>1111</v>
       </c>
       <c r="F70">
         <v>1213</v>
@@ -2889,16 +2676,13 @@
       <c r="J70">
         <v>2019</v>
       </c>
-      <c r="K70">
-        <v>2.840248962655602</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11">
+    </row>
+    <row r="71" spans="1:10">
       <c r="A71" s="1">
         <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C71">
         <v>601</v>
@@ -2907,7 +2691,7 @@
         <v>721</v>
       </c>
       <c r="E71">
-        <v>1597</v>
+        <v>1587</v>
       </c>
       <c r="F71">
         <v>886</v>
@@ -2924,16 +2708,13 @@
       <c r="J71">
         <v>2019</v>
       </c>
-      <c r="K71">
-        <v>0.8335644937586685</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11">
+    </row>
+    <row r="72" spans="1:10">
       <c r="A72" s="1">
         <v>70</v>
       </c>
       <c r="B72" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C72">
         <v>300</v>
@@ -2942,7 +2723,7 @@
         <v>206</v>
       </c>
       <c r="E72">
-        <v>748</v>
+        <v>738</v>
       </c>
       <c r="F72">
         <v>394</v>
@@ -2959,16 +2740,13 @@
       <c r="J72">
         <v>2019</v>
       </c>
-      <c r="K72">
-        <v>1.456310679611651</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11">
+    </row>
+    <row r="73" spans="1:10">
       <c r="A73" s="1">
         <v>71</v>
       </c>
       <c r="B73" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C73">
         <v>198</v>
@@ -2977,7 +2755,7 @@
         <v>126</v>
       </c>
       <c r="E73">
-        <v>367</v>
+        <v>357</v>
       </c>
       <c r="F73">
         <v>234</v>
@@ -2993,9 +2771,6 @@
       </c>
       <c r="J73">
         <v>2019</v>
-      </c>
-      <c r="K73">
-        <v>1.571428571428571</v>
       </c>
     </row>
   </sheetData>

</xml_diff>